<commit_message>
added IO functions for characters and enemies
</commit_message>
<xml_diff>
--- a/data/enemy.xlsx
+++ b/data/enemy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PythonProject\GenshinTeamDPSCalculator\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\PythonProjects\GenshinTeamDPSCalculator\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39BA461F-7AB0-4BB5-AF79-503AABACA9C3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{704F9376-1311-442A-8FE3-7880A1A2C9CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5850" yWindow="3285" windowWidth="21975" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,23 +27,23 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>负二十物抗</t>
+    <t>名称</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>十物抗</t>
+    <t>怪物</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>三十物抗</t>
+    <t>等级</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>五十物抗</t>
+    <t>qq人</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>七十物抗</t>
+    <t>Hilichurl</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -369,10 +369,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -380,179 +380,26 @@
     <col min="1" max="1" width="10.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
-        <v>100</v>
-      </c>
-      <c r="C1">
-        <v>500</v>
-      </c>
-      <c r="D1">
-        <v>0</v>
-      </c>
-      <c r="E1">
-        <v>10</v>
-      </c>
-      <c r="F1">
-        <v>10</v>
-      </c>
-      <c r="G1">
-        <v>10</v>
-      </c>
-      <c r="H1">
-        <v>10</v>
-      </c>
-      <c r="I1">
-        <v>10</v>
-      </c>
-      <c r="J1">
-        <v>10</v>
-      </c>
-      <c r="K1">
-        <v>-20</v>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>100</v>
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
       </c>
       <c r="C2">
-        <v>500</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>10</v>
-      </c>
-      <c r="F2">
-        <v>10</v>
-      </c>
-      <c r="G2">
-        <v>10</v>
-      </c>
-      <c r="H2">
-        <v>10</v>
-      </c>
-      <c r="I2">
-        <v>10</v>
-      </c>
-      <c r="J2">
-        <v>10</v>
-      </c>
-      <c r="K2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>100</v>
-      </c>
-      <c r="C3">
-        <v>500</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>10</v>
-      </c>
-      <c r="F3">
-        <v>10</v>
-      </c>
-      <c r="G3">
-        <v>10</v>
-      </c>
-      <c r="H3">
-        <v>10</v>
-      </c>
-      <c r="I3">
-        <v>10</v>
-      </c>
-      <c r="J3">
-        <v>10</v>
-      </c>
-      <c r="K3">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>100</v>
-      </c>
-      <c r="C4">
-        <v>500</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>10</v>
-      </c>
-      <c r="F4">
-        <v>10</v>
-      </c>
-      <c r="G4">
-        <v>10</v>
-      </c>
-      <c r="H4">
-        <v>10</v>
-      </c>
-      <c r="I4">
-        <v>10</v>
-      </c>
-      <c r="J4">
-        <v>10</v>
-      </c>
-      <c r="K4">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>100</v>
-      </c>
-      <c r="C5">
-        <v>500</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>10</v>
-      </c>
-      <c r="F5">
-        <v>10</v>
-      </c>
-      <c r="G5">
-        <v>10</v>
-      </c>
-      <c r="H5">
-        <v>10</v>
-      </c>
-      <c r="I5">
-        <v>10</v>
-      </c>
-      <c r="J5">
-        <v>10</v>
-      </c>
-      <c r="K5">
-        <v>70</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>